<commit_message>
complete download section both income and expenses
</commit_message>
<xml_diff>
--- a/Backend/income_details.xlsx
+++ b/Backend/income_details.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -416,57 +416,57 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Salary</v>
+        <v>hhh</v>
       </c>
       <c r="B2">
-        <v>114551712000000</v>
+        <v>666</v>
       </c>
       <c r="C2" s="1">
-        <v>45862.22928240741</v>
+        <v>45892.22928240741</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Salary</v>
+        <v>fff</v>
       </c>
       <c r="B3">
-        <v>114551712000000</v>
+        <v>4444</v>
       </c>
       <c r="C3" s="1">
-        <v>45862.22928240741</v>
+        <v>45889.22928240741</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Salary</v>
+        <v xml:space="preserve">Interest </v>
       </c>
       <c r="B4">
-        <v>5600</v>
+        <v>1000</v>
       </c>
       <c r="C4" s="1">
-        <v>45862.22928240741</v>
+        <v>45888.22928240741</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Salary</v>
+        <v>Freelancing</v>
       </c>
       <c r="B5">
-        <v>5600</v>
+        <v>2000</v>
       </c>
       <c r="C5" s="1">
-        <v>45862.22928240741</v>
+        <v>45884.22928240741</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Salary</v>
+        <v>Business Income</v>
       </c>
       <c r="B6">
-        <v>5600</v>
+        <v>6500</v>
       </c>
       <c r="C6" s="1">
-        <v>45862.22928240741</v>
+        <v>45875.22928240741</v>
       </c>
     </row>
     <row r="7">
@@ -474,103 +474,15 @@
         <v>Salary</v>
       </c>
       <c r="B7">
-        <v>7000</v>
+        <v>10000</v>
       </c>
       <c r="C7" s="1">
         <v>45862.22928240741</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Salary</v>
-      </c>
-      <c r="B8">
-        <v>8000</v>
-      </c>
-      <c r="C8" s="1">
-        <v>45862.22928240741</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Salary</v>
-      </c>
-      <c r="B9">
-        <v>8000</v>
-      </c>
-      <c r="C9" s="1">
-        <v>45862.22928240741</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Salary</v>
-      </c>
-      <c r="B10">
-        <v>10000</v>
-      </c>
-      <c r="C10" s="1">
-        <v>45862.22928240741</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>Salary</v>
-      </c>
-      <c r="B11">
-        <v>10000</v>
-      </c>
-      <c r="C11" s="1">
-        <v>45862.22928240741</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>Salary</v>
-      </c>
-      <c r="B12">
-        <v>114551712000000</v>
-      </c>
-      <c r="C12" s="1">
-        <v>45862.86400328704</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>Salary</v>
-      </c>
-      <c r="B13">
-        <v>114551712000000</v>
-      </c>
-      <c r="C13" s="1">
-        <v>45862.86400328704</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>Salary</v>
-      </c>
-      <c r="B14">
-        <v>114551712000000</v>
-      </c>
-      <c r="C14" s="1">
-        <v>45862.86400328704</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>Salary</v>
-      </c>
-      <c r="B15">
-        <v>114551712000000</v>
-      </c>
-      <c r="C15" s="1">
-        <v>45862.86400328704</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>